<commit_message>
working baseline for NemoMod established + mostly complete electricity model
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_se_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_se_demo.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC19C7A7-8F63-A049-9275-897B668CE8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C54582-D978-6B4E-95F4-CFA19C09584F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="460" windowWidth="19900" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
     <sheet name="strategy_id-1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="61">
   <si>
     <t>subsector</t>
   </si>
@@ -195,6 +207,15 @@
   </si>
   <si>
     <t>occrateinit_gnrl_occupancy</t>
+  </si>
+  <si>
+    <t>limit_gnrl_annual_emissions_mt_ch4</t>
+  </si>
+  <si>
+    <t>limit_gnrl_annual_emissions_mt_n2o</t>
+  </si>
+  <si>
+    <t>limit_gnrl_annual_emissions_mt_co2</t>
   </si>
 </sst>
 </file>
@@ -596,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS12"/>
+  <dimension ref="A1:AS15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AQ15" sqref="AQ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2081,6 +2102,372 @@
       </c>
       <c r="AS12">
         <v>3.145207224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>-999</v>
+      </c>
+      <c r="K13">
+        <v>-999</v>
+      </c>
+      <c r="L13">
+        <v>-999</v>
+      </c>
+      <c r="M13">
+        <v>-999</v>
+      </c>
+      <c r="N13">
+        <v>-999</v>
+      </c>
+      <c r="O13">
+        <v>-999</v>
+      </c>
+      <c r="P13">
+        <v>-999</v>
+      </c>
+      <c r="Q13">
+        <v>-999</v>
+      </c>
+      <c r="R13">
+        <v>-999</v>
+      </c>
+      <c r="S13">
+        <v>-999</v>
+      </c>
+      <c r="T13">
+        <v>-999</v>
+      </c>
+      <c r="U13">
+        <v>-999</v>
+      </c>
+      <c r="V13">
+        <v>-999</v>
+      </c>
+      <c r="W13">
+        <v>-999</v>
+      </c>
+      <c r="X13">
+        <v>-999</v>
+      </c>
+      <c r="Y13">
+        <v>-999</v>
+      </c>
+      <c r="Z13">
+        <v>-999</v>
+      </c>
+      <c r="AA13">
+        <v>-999</v>
+      </c>
+      <c r="AB13">
+        <v>-999</v>
+      </c>
+      <c r="AC13">
+        <v>-999</v>
+      </c>
+      <c r="AD13">
+        <v>-999</v>
+      </c>
+      <c r="AE13">
+        <v>-999</v>
+      </c>
+      <c r="AF13">
+        <v>-999</v>
+      </c>
+      <c r="AG13">
+        <v>-999</v>
+      </c>
+      <c r="AH13">
+        <v>-999</v>
+      </c>
+      <c r="AI13">
+        <v>-999</v>
+      </c>
+      <c r="AJ13">
+        <v>-999</v>
+      </c>
+      <c r="AK13">
+        <v>-999</v>
+      </c>
+      <c r="AL13">
+        <v>-999</v>
+      </c>
+      <c r="AM13">
+        <v>-999</v>
+      </c>
+      <c r="AN13">
+        <v>-999</v>
+      </c>
+      <c r="AO13">
+        <v>-999</v>
+      </c>
+      <c r="AP13">
+        <v>-999</v>
+      </c>
+      <c r="AQ13">
+        <v>-999</v>
+      </c>
+      <c r="AR13">
+        <v>-999</v>
+      </c>
+      <c r="AS13">
+        <v>-999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>-999</v>
+      </c>
+      <c r="K14">
+        <v>-999</v>
+      </c>
+      <c r="L14">
+        <v>-999</v>
+      </c>
+      <c r="M14">
+        <v>-999</v>
+      </c>
+      <c r="N14">
+        <v>-999</v>
+      </c>
+      <c r="O14">
+        <v>-999</v>
+      </c>
+      <c r="P14">
+        <v>-999</v>
+      </c>
+      <c r="Q14">
+        <v>-999</v>
+      </c>
+      <c r="R14">
+        <v>-999</v>
+      </c>
+      <c r="S14">
+        <v>-999</v>
+      </c>
+      <c r="T14">
+        <v>-999</v>
+      </c>
+      <c r="U14">
+        <v>-999</v>
+      </c>
+      <c r="V14">
+        <v>-999</v>
+      </c>
+      <c r="W14">
+        <v>-999</v>
+      </c>
+      <c r="X14">
+        <v>-999</v>
+      </c>
+      <c r="Y14">
+        <v>-999</v>
+      </c>
+      <c r="Z14">
+        <v>-999</v>
+      </c>
+      <c r="AA14">
+        <v>-999</v>
+      </c>
+      <c r="AB14">
+        <v>-999</v>
+      </c>
+      <c r="AC14">
+        <v>-999</v>
+      </c>
+      <c r="AD14">
+        <v>-999</v>
+      </c>
+      <c r="AE14">
+        <v>-999</v>
+      </c>
+      <c r="AF14">
+        <v>-999</v>
+      </c>
+      <c r="AG14">
+        <v>-999</v>
+      </c>
+      <c r="AH14">
+        <v>-999</v>
+      </c>
+      <c r="AI14">
+        <v>-999</v>
+      </c>
+      <c r="AJ14">
+        <v>-999</v>
+      </c>
+      <c r="AK14">
+        <v>-999</v>
+      </c>
+      <c r="AL14">
+        <v>-999</v>
+      </c>
+      <c r="AM14">
+        <v>-999</v>
+      </c>
+      <c r="AN14">
+        <v>-999</v>
+      </c>
+      <c r="AO14">
+        <v>-999</v>
+      </c>
+      <c r="AP14">
+        <v>-999</v>
+      </c>
+      <c r="AQ14">
+        <v>-999</v>
+      </c>
+      <c r="AR14">
+        <v>-999</v>
+      </c>
+      <c r="AS14">
+        <v>-999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>-999</v>
+      </c>
+      <c r="K15">
+        <v>-999</v>
+      </c>
+      <c r="L15">
+        <v>-999</v>
+      </c>
+      <c r="M15">
+        <v>-999</v>
+      </c>
+      <c r="N15">
+        <v>-999</v>
+      </c>
+      <c r="O15">
+        <v>-999</v>
+      </c>
+      <c r="P15">
+        <v>-999</v>
+      </c>
+      <c r="Q15">
+        <v>-999</v>
+      </c>
+      <c r="R15">
+        <v>-999</v>
+      </c>
+      <c r="S15">
+        <v>-999</v>
+      </c>
+      <c r="T15">
+        <v>-999</v>
+      </c>
+      <c r="U15">
+        <v>-999</v>
+      </c>
+      <c r="V15">
+        <v>-999</v>
+      </c>
+      <c r="W15">
+        <v>-999</v>
+      </c>
+      <c r="X15">
+        <v>-999</v>
+      </c>
+      <c r="Y15">
+        <v>-999</v>
+      </c>
+      <c r="Z15">
+        <v>-999</v>
+      </c>
+      <c r="AA15">
+        <v>-999</v>
+      </c>
+      <c r="AB15">
+        <v>-999</v>
+      </c>
+      <c r="AC15">
+        <v>-999</v>
+      </c>
+      <c r="AD15">
+        <v>-999</v>
+      </c>
+      <c r="AE15">
+        <v>-999</v>
+      </c>
+      <c r="AF15">
+        <v>-999</v>
+      </c>
+      <c r="AG15">
+        <v>-999</v>
+      </c>
+      <c r="AH15">
+        <v>-999</v>
+      </c>
+      <c r="AI15">
+        <v>-999</v>
+      </c>
+      <c r="AJ15">
+        <v>-999</v>
+      </c>
+      <c r="AK15">
+        <v>-999</v>
+      </c>
+      <c r="AL15">
+        <v>-999</v>
+      </c>
+      <c r="AM15">
+        <v>-999</v>
+      </c>
+      <c r="AN15">
+        <v>-999</v>
+      </c>
+      <c r="AO15">
+        <v>-999</v>
+      </c>
+      <c r="AP15">
+        <v>-999</v>
+      </c>
+      <c r="AQ15">
+        <v>-999</v>
+      </c>
+      <c r="AR15">
+        <v>-999</v>
+      </c>
+      <c r="AS15">
+        <v>-999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>